<commit_message>
Vælg tidspunkt fra listbox.
</commit_message>
<xml_diff>
--- a/SensorDataFil.xlsx
+++ b/SensorDataFil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruger\Documents\Bachelorprojekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\Sundhedsteknologi\7. Semester\Bachelor\MatLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A6D2BC85-48C0-40E5-B651-7BAA0C899A50}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AEEF85C0-C4AE-461D-8604-E315026B3589}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9070" xr2:uid="{67E6E48D-6249-4DA5-9873-57FE481732B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{67E6E48D-6249-4DA5-9873-57FE481732B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Varighed for arbejdsgang</t>
+  </si>
+  <si>
+    <t>10.23</t>
+  </si>
+  <si>
+    <t>00.40</t>
   </si>
 </sst>
 </file>
@@ -496,21 +502,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D3C2A-ED3E-4A0E-BC8A-DBBB57E283BF}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -586,7 +592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -624,7 +630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
@@ -662,7 +668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -700,7 +706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -738,7 +744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -776,7 +782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -814,7 +820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -852,7 +858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -890,7 +896,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -928,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -966,7 +972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1040,6 +1046,44 @@
       </c>
       <c r="L14" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43382.772916666669</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Billede af Luna og Carendo på "Valgt af teknologi" og SensorData-fil er opdateret med nye kategorier
</commit_message>
<xml_diff>
--- a/SensorDataFil.xlsx
+++ b/SensorDataFil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruger\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\Sundhedsteknologi\7. Semester\Bachelor\MatLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E90F477-2271-48DC-8EE5-424DE9F03C07}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22C34605-32E2-4CD1-A31F-795AD4EA0AAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9070" xr2:uid="{67E6E48D-6249-4DA5-9873-57FE481732B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{67E6E48D-6249-4DA5-9873-57FE481732B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -54,15 +54,6 @@
     <t>Anvendelse af luna sammen med Carendo</t>
   </si>
   <si>
-    <t>10.57</t>
-  </si>
-  <si>
-    <t>05.05</t>
-  </si>
-  <si>
-    <t>04.33</t>
-  </si>
-  <si>
     <t>Arbejdsgang</t>
   </si>
   <si>
@@ -87,54 +78,27 @@
     <t>02.56</t>
   </si>
   <si>
-    <t>Personalefaglighed</t>
-  </si>
-  <si>
-    <t>Alm</t>
-  </si>
-  <si>
     <t>Superbruger</t>
   </si>
   <si>
-    <t>06.58</t>
-  </si>
-  <si>
     <t>03.02</t>
   </si>
   <si>
-    <t>07.05</t>
-  </si>
-  <si>
     <t>02.05</t>
   </si>
   <si>
-    <t>11.35</t>
-  </si>
-  <si>
     <t>03.55</t>
   </si>
   <si>
-    <t>08.53</t>
-  </si>
-  <si>
     <t>02.35</t>
   </si>
   <si>
-    <t>09.05</t>
-  </si>
-  <si>
     <t>01.52</t>
   </si>
   <si>
-    <t>10.25</t>
-  </si>
-  <si>
     <t>Aftenhygijne</t>
   </si>
   <si>
-    <t>15.35</t>
-  </si>
-  <si>
     <t>03.05</t>
   </si>
   <si>
@@ -144,10 +108,25 @@
     <t>Varighed for arbejdsgang</t>
   </si>
   <si>
-    <t>10.33</t>
-  </si>
-  <si>
     <t>00.30</t>
+  </si>
+  <si>
+    <t>Almindeligt personale</t>
+  </si>
+  <si>
+    <t>Afløser</t>
+  </si>
+  <si>
+    <t>Varighed m. 2+ medarbejdere</t>
+  </si>
+  <si>
+    <t>Varighed m. 1 medarbejder</t>
+  </si>
+  <si>
+    <t>Varighed m. 0 medarbejder</t>
+  </si>
+  <si>
+    <t>Datasæt med rådata</t>
   </si>
 </sst>
 </file>
@@ -502,21 +481,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D3C2A-ED3E-4A0E-BC8A-DBBB57E283BF}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,22 +518,40 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -576,23 +573,38 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
+      <c r="H2" s="3">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -614,23 +626,38 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>37</v>
+      <c r="H3" s="3">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
@@ -652,23 +679,38 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
+      <c r="H4" s="3">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -690,23 +732,38 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>24</v>
+      <c r="H5" s="3">
+        <v>0.2902777777777778</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.12361111111111112</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -728,23 +785,38 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>26</v>
+      <c r="H6" s="3">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="I6" s="3">
+        <v>7</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -766,23 +838,38 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
+      <c r="H7" s="3">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -804,23 +891,38 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>30</v>
+      <c r="H8" s="3">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
       </c>
       <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -842,23 +944,38 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>24</v>
+      <c r="H9" s="3">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="I9" s="3">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -880,23 +997,38 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>32</v>
+      <c r="H10" s="3">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -918,23 +1050,38 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
+      <c r="H11" s="3">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
       </c>
       <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -956,23 +1103,38 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>36</v>
+      <c r="H12" s="3">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -994,23 +1156,38 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>36</v>
+      <c r="H13" s="3">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1032,20 +1209,35 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>40</v>
+      <c r="H14" s="3">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.35625000000000001</v>
+      </c>
+      <c r="J14" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SammenlignMedPlejeCentre og yderligere Data påbegyndt
</commit_message>
<xml_diff>
--- a/SensorDataFil.xlsx
+++ b/SensorDataFil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruger\Documents\Bachelorprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F9CAAFE4-B982-4E40-A5AC-AA66DCFDACF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A4B30191-8A58-46F9-9526-4FF1B85880B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9070" xr2:uid="{67E6E48D-6249-4DA5-9873-57FE481732B7}"/>
   </bookViews>
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D3C2A-ED3E-4A0E-BC8A-DBBB57E283BF}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1342,6 +1342,9 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I16" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Yderligere Data er fikset og sensorfil har ikke to kolonner længere
</commit_message>
<xml_diff>
--- a/SensorDataFil.xlsx
+++ b/SensorDataFil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruger\Documents\Bachelorprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A4B30191-8A58-46F9-9526-4FF1B85880B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91B67977-9D20-40C5-A88C-C2B11CE63756}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9070" xr2:uid="{67E6E48D-6249-4DA5-9873-57FE481732B7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Hæve sænke funktion</t>
-  </si>
-  <si>
-    <t>Anvendelse af luna sammen med Carendo</t>
   </si>
   <si>
     <t>Arbejdsgang</t>
@@ -541,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D3C2A-ED3E-4A0E-BC8A-DBBB57E283BF}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,7 +552,7 @@
     <col min="6" max="6" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,13 +572,13 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
         <v>30</v>
@@ -590,31 +587,28 @@
         <v>31</v>
       </c>
       <c r="L1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="Q1" t="s">
         <v>28</v>
       </c>
       <c r="R1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -636,41 +630,38 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
+      <c r="H2" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2">
         <v>2</v>
       </c>
-      <c r="O2" t="s">
-        <v>15</v>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -690,43 +681,40 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3">
         <v>2</v>
       </c>
-      <c r="O3" t="s">
-        <v>25</v>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
         <v>1</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
@@ -746,43 +734,40 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -804,41 +789,38 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="H5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5">
         <v>2</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>18</v>
+      <c r="N5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -858,43 +840,40 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -914,43 +893,40 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7" t="s">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -970,43 +946,40 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N8">
+        <v>44</v>
+      </c>
+      <c r="L8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8">
         <v>2</v>
       </c>
-      <c r="O8" t="s">
-        <v>21</v>
+      <c r="N8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>1</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1028,41 +1001,38 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>0</v>
+      <c r="H9" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>18</v>
+        <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1084,41 +1054,38 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>0</v>
+      <c r="H10" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10" t="s">
-        <v>22</v>
+        <v>44</v>
+      </c>
+      <c r="L10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1140,41 +1107,38 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>0</v>
+      <c r="H11" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1196,41 +1160,38 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <v>0</v>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="L12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1252,41 +1213,38 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>0</v>
+      <c r="H13" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="L13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1308,41 +1266,38 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <v>0</v>
+      <c r="H14" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I16" s="3"/>
     </row>
   </sheetData>

</xml_diff>